<commit_message>
Updating documents from invoices for December
</commit_message>
<xml_diff>
--- a/Asset Registry System (ARS)/ARS Requirements Phase 3 work_V22.xlsx
+++ b/Asset Registry System (ARS)/ARS Requirements Phase 3 work_V22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/btw897_ku_dk/Documents/DaSSCo-Tranche-1-work/Asset Registry System (ARS)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{B245CD1A-D358-4CAE-8D69-48AFBC9E5966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7617789-D649-4E63-BDEC-9F7E45FF77C3}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{B245CD1A-D358-4CAE-8D69-48AFBC9E5966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{080665FF-1590-4471-9091-ABB85DE98B24}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E45C9BED-A893-4BAC-8B4F-82BC01806C6A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{E45C9BED-A893-4BAC-8B4F-82BC01806C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1527,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1585,6 +1585,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1626,11 +1627,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Pip Brewer" refreshedDate="45637.449330324074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="131" xr:uid="{4BFC3A95-E330-4D4E-B05B-22632AD2FC81}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Pip Brewer" refreshedDate="45671.623083101855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="131" xr:uid="{4BFC3A95-E330-4D4E-B05B-22632AD2FC81}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:N1048576" sheet="Main"/>
   </cacheSource>
-  <cacheFields count="15">
+  <cacheFields count="14">
     <cacheField name="#" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
@@ -1655,10 +1656,10 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="DaSSCo Agreed Date" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2023-12-20T00:00:00" maxDate="2024-11-21T00:00:00"/>
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2023-12-20T00:00:00" maxDate="2024-11-21T00:00:00"/>
     </cacheField>
     <cacheField name="Date Communicated to NT" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2024-06-10T00:00:00" maxDate="2024-06-24T00:00:00"/>
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2024-06-10T00:00:00" maxDate="2024-06-24T00:00:00"/>
     </cacheField>
     <cacheField name="NT Hours Predicted" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="35"/>
@@ -1669,20 +1670,17 @@
     <cacheField name="NHMD Priority" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
     </cacheField>
-    <cacheField name="Issue" numFmtId="0">
-      <sharedItems containsBlank="1" longText="1"/>
-    </cacheField>
     <cacheField name="Github ticket" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Completed Date" numFmtId="0">
-      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2024-05-15T00:00:00" maxDate="2024-12-10T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2024-05-15T00:00:00" maxDate="2024-12-10T00:00:00"/>
     </cacheField>
     <cacheField name="Notes" numFmtId="0">
       <sharedItems containsBlank="1" longText="1"/>
     </cacheField>
     <cacheField name="ARS Version" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
     </cacheField>
     <cacheField name="Reason" numFmtId="0">
       <sharedItems containsBlank="1" longText="1"/>
@@ -1699,6 +1697,38 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="131">
   <r>
+    <s v="R1.12"/>
+    <s v="Provide status for each asset via request"/>
+    <x v="0"/>
+    <s v="Completed"/>
+    <d v="2023-12-20T00:00:00"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <n v="1"/>
+    <s v="#45_x000a_#81"/>
+    <m/>
+    <s v="Bug as sometimes showing faulty information about the status. _x000a_In icebox"/>
+    <m/>
+    <s v="Let us know where in the ARS part of the pipeline an asset is. It allows us to see errors, succesful creation of asset/files, persist status and storage space used. "/>
+  </r>
+  <r>
+    <s v="R1.13"/>
+    <s v="Sync the asset with ERDA"/>
+    <x v="0"/>
+    <s v="Completed"/>
+    <d v="2023-12-20T00:00:00"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="Bug 504 for open shares, need to extend timeout limits on nginx by us_x000a_In icebox"/>
+    <m/>
+    <s v="Since uploading files to ERDA is not done in a single flow we need a way to verify that the files were pushed successfully. There have been several issues with ERDA connection, including issues with unstability, not checking if the connections had died off, had to put a delay to establish simultaneous connections"/>
+  </r>
+  <r>
     <s v="R1.003"/>
     <s v="Change allocated space when downloading it from ERDA into file proxy incase the asset needs more space / has parent attached to it"/>
     <x v="0"/>
@@ -1709,7 +1739,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1726,7 +1755,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1743,7 +1771,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1760,7 +1787,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1777,7 +1803,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1794,7 +1819,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Still not working"/>
     <m/>
@@ -1811,7 +1835,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-06-16T00:00:00"/>
     <s v="There was an issue with the way integrity check was done, they never rejected the file if it was curropt but later it was corrected"/>
     <m/>
@@ -1828,7 +1851,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Later it was extended to be able to delete file from ERDA also, related to R3.12"/>
     <m/>
@@ -1845,7 +1867,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1863,10 +1884,25 @@
     <m/>
     <m/>
     <m/>
-    <s v="related to R1.8"/>
-    <s v="Initially, the functionality was that we would provide,messageintegrity(CRC), while uploading a file and ARS would be checked against the CRC of received file, but no action would be taken, then it was requested to delete the corrupt file and send a message back that file was not persisted. Date missing."/>
+    <s v="Initially, the functionality was that we would provide,messageintegrity(CRC), while uploading a file and ARS would be checked against the CRC of received file, but no action would be taken, then it was requested to delete the corrupt file and send a message back that file was not persisted. Date missing._x000a_Related to R1.8"/>
     <m/>
     <s v="To check if the file was succesfuly uploaded and to help us keep track of storage space used by the fileproxy. Also helps us determine if we have correctly received the file for processing."/>
+  </r>
+  <r>
+    <s v="R1.14"/>
+    <s v="See all the assets currently being worked on, and their status"/>
+    <x v="0"/>
+    <s v="Completed"/>
+    <d v="2023-12-20T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2024-05-15T00:00:00"/>
+    <s v="Created a new requirement for including the status in Get list shares end point_x000a_Same version after cleaning DB"/>
+    <m/>
+    <s v="Gives an overview of assets in the ARS part of the pipeline. Lets us quickly find assets that for some reason have had their progress halted. "/>
   </r>
   <r>
     <s v="R1.15"/>
@@ -1879,7 +1915,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1896,7 +1931,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Parent was always checked out, but optimisation was requested, where only when parent guid was filled out when creating asset then, ERDA would be connected to get parent asset. Was part of first testing iteration, notes in GitHub"/>
     <m/>
@@ -1913,7 +1947,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Partially achieved, rest dropped. Some specifics are part of other requirements listed here."/>
     <m/>
@@ -1930,7 +1963,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <m/>
     <m/>
@@ -1947,62 +1979,10 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Related to R3.12"/>
     <m/>
     <m/>
-  </r>
-  <r>
-    <s v="R1.12"/>
-    <s v="Provide status for each asset via request"/>
-    <x v="0"/>
-    <s v="Completed"/>
-    <d v="2023-12-20T00:00:00"/>
-    <m/>
-    <m/>
-    <n v="1"/>
-    <n v="1"/>
-    <m/>
-    <s v="#45_x000a_#81"/>
-    <s v="in icebox"/>
-    <s v="Bug as sometimes showing faulty information about the status. "/>
-    <m/>
-    <s v="Let us know where in the ARS part of the pipeline an asset is. It allows us to see errors, succesful creation of asset/files, persist status and storage space used. "/>
-  </r>
-  <r>
-    <s v="R1.13"/>
-    <s v="Sync the asset with ERDA"/>
-    <x v="0"/>
-    <s v="Completed"/>
-    <d v="2023-12-20T00:00:00"/>
-    <m/>
-    <m/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="in icebox"/>
-    <s v="Bug 504 for open shares, need to extend timeout limits on nginx by us"/>
-    <m/>
-    <s v="Since uploading files to ERDA is not done in a single flow we need a way to verify that the files were pushed successfully. There have been several issues with ERDA connection, including issues with unstability, not checking if the connections had died off, had to put a delay to establish simultaneous connections"/>
-  </r>
-  <r>
-    <s v="R1.14"/>
-    <s v="See all the assets currently being worked on, and their status"/>
-    <x v="0"/>
-    <s v="Completed"/>
-    <d v="2023-12-20T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <d v="2024-05-15T00:00:00"/>
-    <s v="created a new requirement for including the status in Get list shares end point"/>
-    <s v="same version after cleaning DB"/>
-    <s v="Gives an overview of assets in the ARS part of the pipeline. Lets us quickly find assets that for some reason have had their progress halted. "/>
   </r>
   <r>
     <s v="R1.17"/>
@@ -2014,7 +1994,6 @@
     <n v="8"/>
     <n v="3"/>
     <m/>
-    <m/>
     <s v="#43"/>
     <m/>
     <s v="Moved this to low priority"/>
@@ -2031,10 +2010,9 @@
     <n v="3"/>
     <n v="3"/>
     <n v="2"/>
-    <m/>
     <s v="#35"/>
-    <s v="related to R1.7"/>
-    <s v="We have scalable solutions for deployment in DeIC and Docker, R 3.17 also adresses the same. The suggested sol needs to be tested by us. We need to ask NT, how to replace   ERDA or add another storage with sftp to ARS - maybe in next agreement"/>
+    <m/>
+    <s v="We have scalable solutions for deployment in DeIC and Docker. R 3.17 also adresses the same. The suggested solution needs to be tested by us. We need to ask NT, how to replace ERDA or add another storage with sftp to ARS - maybe in next agreement._x000a_Related to R1.7."/>
     <m/>
     <s v="This is not explicitly mentioned in WP1 but is part of the requirement, but was the core requirement of previous work and changing to HTTP as part of initial discussion, lilke other several requirements which are presumed to be part of this WP1, as this work package only specific on change of protocol "/>
   </r>
@@ -2048,10 +2026,9 @@
     <n v="8"/>
     <n v="3"/>
     <n v="2"/>
-    <m/>
     <s v="#43"/>
     <m/>
-    <s v="Same as R1.14, moved to low priority"/>
+    <s v="Same as R1.14. Moved to low priority"/>
     <m/>
     <s v="This requirement partially addresed the scalability and extensibility  requirement "/>
   </r>
@@ -2065,12 +2042,43 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="#43"/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Part of status in WP1"/>
     <m/>
     <m/>
+  </r>
+  <r>
+    <s v="R3.08"/>
+    <s v="Provide endpoints to update access control to institutions, collections on the existing API"/>
+    <x v="1"/>
+    <s v="Completed"/>
+    <d v="2024-02-20T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="#100"/>
+    <m/>
+    <s v="Documentation/swagger doesnt show how but in meeting with Christoffer and Thomas, we have in github, Need to be implemented and better documented by us"/>
+    <m/>
+    <s v="testing what is needed "/>
+  </r>
+  <r>
+    <s v="R3.11"/>
+    <s v="It should be possible to give role-based access to assets, collections, institutions, e.g. the digitiser can have access to certain collections they are working on, and not have access to the rest"/>
+    <x v="1"/>
+    <s v="Completed"/>
+    <d v="2024-02-20T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="Achieved for institution level and collection level in WP5A, post poned the rest, needs testing by us in keycloak and documentation update needed."/>
+    <m/>
+    <s v="current status of documentation https://github.com/NHMDenmark/DaSSCo-asset-service/blob/main/documentation/confluence-docs/role-based-access-control.md"/>
   </r>
   <r>
     <s v="R3.12 - part"/>
@@ -2083,7 +2091,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Covered by WP1 for assets- we can delete share including the files in the share in fileproxy to clean up space, and also delete files in ERDA is a peculiar way just incase. when deleting a file it doesn't update the delete_file_After_sync: assuming this a way to keep track of all files that existed for an asset but bug in functionality. This works for Northtech, but not us (other than assets - which we can)."/>
     <m/>
@@ -2100,7 +2107,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-08-15T00:00:00"/>
     <s v="Requested during deployment. Needs investigation for ucloud deployment."/>
     <m/>
@@ -2117,7 +2123,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-08-15T00:00:00"/>
     <s v="Requested during deployment. Needs investigation for ucloud deployment."/>
     <m/>
@@ -2130,13 +2135,12 @@
     <s v="In progress"/>
     <d v="2024-02-20T00:00:00"/>
     <m/>
-    <m/>
+    <n v="0"/>
     <n v="1"/>
     <n v="1"/>
-    <m/>
     <s v="#104"/>
     <d v="2024-09-06T00:00:00"/>
-    <s v="We have tested it, some documentation is missing"/>
+    <s v="We have tested it, some documentation is missing. The number of NT hours to complete this is included under 3.9."/>
     <m/>
     <s v="Covered by API provided for search functionality in WP5A"/>
   </r>
@@ -2150,10 +2154,57 @@
     <n v="20"/>
     <n v="1"/>
     <m/>
-    <m/>
     <s v="#104"/>
     <m/>
     <s v="We have tested it, some documentation is missing, some metadata fields missing which will come after our metadata update request like last_updated_by"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R3.09"/>
+    <s v="Update API documentation of mandatory parameters and document API requests with examples."/>
+    <x v="1"/>
+    <s v="In progress"/>
+    <d v="2024-02-20T00:00:00"/>
+    <m/>
+    <n v="15"/>
+    <n v="1"/>
+    <m/>
+    <s v="#104"/>
+    <m/>
+    <s v="Issues with update end points and some depricated end points still in the docs, look at, some documentation is missing"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R3.15"/>
+    <s v="Provide documentation on different work flows between file proxy and ARS and ERDA, specifically the difference between the work flow for UI and API, WP2A work flow documentation, various caches, etc"/>
+    <x v="1"/>
+    <s v="In progress"/>
+    <d v="2024-02-20T00:00:00"/>
+    <m/>
+    <n v="10"/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="We have some diagrams. Still missing various workflows from asset service to file proxy. Can wait until WP2A is done - would like them to do this one for what they have until now - not in github yet"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R3.17"/>
+    <s v="Provide help/suggestions on automation of scalability"/>
+    <x v="1"/>
+    <s v="In progress"/>
+    <d v="2024-02-20T00:00:00"/>
+    <m/>
+    <n v="4"/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="We can do the rest ourselves, if needed, 3-4 hrs of christoffers help will be enough.We have scalability solutions for DeIC deployment and docker deployment, I hve to test if it works…and document it, need insights on replacing ERDA"/>
     <m/>
     <m/>
   </r>
@@ -2168,79 +2219,10 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <s v="Needs testing - part of WP2A and metadata discussion - needs to wait until WP2A is done"/>
     <m/>
     <s v="Search API from WP5A provides that, belongs in WP2A"/>
-  </r>
-  <r>
-    <s v="R3.08"/>
-    <s v="Provide endpoints to update access control to institutions, collections on the existing API"/>
-    <x v="1"/>
-    <s v="Completed"/>
-    <d v="2024-02-20T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="#100"/>
-    <m/>
-    <s v="Documentation/swagger doesnt show how but in meeting with Christoffer and Thomas, we have in github, Need to be implemented and better documented by us"/>
-    <m/>
-    <s v="testing what is needed "/>
-  </r>
-  <r>
-    <s v="R3.09"/>
-    <s v="Update API documentation of mandatory parameters and document API requests with examples."/>
-    <x v="1"/>
-    <s v="In progress"/>
-    <d v="2024-02-20T00:00:00"/>
-    <m/>
-    <n v="15"/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <s v="#104"/>
-    <m/>
-    <s v="Issues with update end points and some depricated end pointsstill in the docs, look at, some documentation is missing"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="R3.11"/>
-    <s v="It should be possible to give role-based access to assets, collections, institutions, e.g. the digitiser can have access to certain collections they are working on, and not have access to the rest"/>
-    <x v="1"/>
-    <s v="Completed"/>
-    <d v="2024-02-20T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="Achieved for institution level and collection level in WP5A, post poned the rest, needs testing by us in keycloak and documentation update needed."/>
-    <m/>
-    <s v="current status of documentation https://github.com/NHMDenmark/DaSSCo-asset-service/blob/main/documentation/confluence-docs/role-based-access-control.md"/>
-  </r>
-  <r>
-    <s v="R3.15"/>
-    <s v="Provide documentation on different work flows between file proxy and ARS and ERDA, specifically the difference between the work flow for UI and API, WP2A work flow documentation, various caches, etc"/>
-    <x v="1"/>
-    <s v="In progress"/>
-    <d v="2024-02-20T00:00:00"/>
-    <m/>
-    <n v="10"/>
-    <n v="2"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="We have some diagrams. Still missing various workflows from asset service to file proxy. Can wait until WP2A is done - would like them to do this one for what they have until now - not in github yet"/>
-    <m/>
-    <m/>
   </r>
   <r>
     <s v="R3.16"/>
@@ -2249,8 +2231,7 @@
     <s v="In progress"/>
     <d v="2024-02-20T00:00:00"/>
     <m/>
-    <m/>
-    <m/>
+    <n v="0"/>
     <m/>
     <m/>
     <m/>
@@ -2260,19 +2241,18 @@
     <m/>
   </r>
   <r>
-    <s v="R3.17"/>
-    <s v="Provide help/suggestions on automation of scalability"/>
+    <s v="R3.20"/>
+    <s v="Deploy test suite"/>
     <x v="1"/>
-    <s v="In progress"/>
-    <d v="2024-02-20T00:00:00"/>
-    <m/>
-    <n v="4"/>
-    <n v="2"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="We can do the rest ourselves, if needed, 3-4 hrs of christoffers help will be enough.We have scalability solutions for DeIC deployment and docker deployment, I hve to test if it works…and document it, need insights on replacing ERDA"/>
+    <s v="Not started"/>
+    <d v="2024-11-20T00:00:00"/>
+    <m/>
+    <n v="10"/>
+    <n v="1"/>
+    <m/>
+    <s v="#105_x000a_#106"/>
+    <m/>
+    <m/>
     <m/>
     <m/>
   </r>
@@ -2291,7 +2271,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R3.10"/>
@@ -2305,7 +2284,6 @@
     <m/>
     <m/>
     <m/>
-    <s v="Edit"/>
     <s v="Achieved for institution level and collection level in WP5A, post poned the rest "/>
     <m/>
     <m/>
@@ -2322,7 +2300,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="On going-inital bugs were fixed "/>
     <m/>
     <m/>
@@ -2338,7 +2315,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-05-15T00:00:00"/>
     <s v="Covered by WP1 for assets- we can delete share including the files in the share in fileproxy to clean up space, and also delete files in ERDA is a peculiar way just incase. when deleting a file it doesn't update the delete_file_After_sync: assuming this a way to keep track of all files that existed for an asset but bug in functionality. We are able to delete assets, but"/>
     <m/>
@@ -2359,7 +2335,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.02"/>
@@ -2376,7 +2351,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.03"/>
@@ -2393,7 +2367,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.04"/>
@@ -2410,7 +2383,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.05"/>
@@ -2427,7 +2399,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.06"/>
@@ -2444,7 +2415,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.07"/>
@@ -2461,7 +2431,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R4.08"/>
@@ -2469,7 +2438,6 @@
     <x v="2"/>
     <m/>
     <d v="2024-02-20T00:00:00"/>
-    <m/>
     <m/>
     <m/>
     <m/>
@@ -2494,7 +2462,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Needed to decide for how Specify, it was already possible to have multiple files for an asset and on recommendation fo NT it was decided that thumbnails will be part of an asset"/>
   </r>
   <r>
@@ -2511,7 +2478,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="To develop a specify adapter that can and crete new attachment record for the existing collection object in specify and add certain metadata from ARS to specify, and Send attachment file from ARS and save in Specify for the newly added attachment record in specify"/>
   </r>
   <r>
@@ -2529,7 +2495,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2A.04"/>
@@ -2546,7 +2511,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2A.05"/>
@@ -2560,7 +2524,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Using message queues in the specify adapter which is able to receive new assets, updates for synced assets and then make relevant calls in the Specify API for synchronisation"/>
     <m/>
     <m/>
@@ -2580,7 +2543,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2A.09"/>
@@ -2597,7 +2559,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2A.07"/>
@@ -2614,7 +2575,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2A.08"/>
@@ -2628,7 +2588,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="This will be revisited when web asset server is replaced, it will become relevant then, because now Specify/webasset server is generating thumbnails"/>
     <m/>
     <m/>
@@ -2648,7 +2607,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2665,7 +2623,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2682,7 +2639,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2699,7 +2655,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2716,7 +2671,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2733,7 +2687,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2B.01"/>
@@ -2750,7 +2703,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.01"/>
@@ -2767,7 +2719,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.02"/>
@@ -2784,7 +2735,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.03"/>
@@ -2801,7 +2751,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.04"/>
@@ -2818,7 +2767,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.05"/>
@@ -2835,7 +2783,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.06"/>
@@ -2852,7 +2799,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R2C.07"/>
@@ -2869,7 +2815,54 @@
     <m/>
     <m/>
     <m/>
-    <m/>
+  </r>
+  <r>
+    <s v="R3.19"/>
+    <s v="Provide granular control over access at  institution and collection level. "/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-30T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2024-12-09T00:00:00"/>
+    <s v="Documentation of this is  https://github.com/NHMDenmark/DaSSCo-asset-service/issues/100, needs testing by us"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R5A.11"/>
+    <s v="In detailed view, it is possible to navigate back and forth through assets that have been retrieved as part of a search. "/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2024-09-24T00:00:00"/>
+    <m/>
+    <m/>
+    <s v="To see the search result in a sequence for inspection or other purposes"/>
+  </r>
+  <r>
+    <s v="R5A.13"/>
+    <s v="It is possible to create a group of asset records and add to this group with additional records later.  "/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <d v="2024-09-24T00:00:00"/>
+    <m/>
+    <m/>
+    <s v="To save search results and maintain/add to them for purpose of correction, bulk action, or similar"/>
   </r>
   <r>
     <s v="R5A.17"/>
@@ -2882,7 +2875,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-24T00:00:00"/>
     <m/>
     <m/>
@@ -2899,11 +2891,42 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-24T00:00:00"/>
     <m/>
     <m/>
     <s v="Part of add to search functionality"/>
+  </r>
+  <r>
+    <s v="R5A.24"/>
+    <s v="It should be possible to assign either write or read only access to pre-defined users of ARS, who are able to log in and view records using the UI"/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <s v="#102"/>
+    <d v="2024-12-09T00:00:00"/>
+    <s v="Graph issue"/>
+    <m/>
+    <s v="Allow a limited number of people to use it and try it out (due to lack of may security features most people will have only read access)"/>
+  </r>
+  <r>
+    <s v="R5A.25"/>
+    <s v="It should be possible to download graphs and statistics in the dashboard view as reports and PDFs/editable documents. "/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <s v="#102"/>
+    <d v="2024-12-09T00:00:00"/>
+    <s v="Graph issue"/>
+    <m/>
+    <s v="Exisitng functionality, updated to support new features"/>
   </r>
   <r>
     <s v="R5A.30"/>
@@ -2916,7 +2939,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <m/>
     <m/>
@@ -2936,25 +2958,7 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Not sure if this is a requirement"/>
-  </r>
-  <r>
-    <s v="R5A.33"/>
-    <s v="The assets are visible in the UI in the form of both a list view and detailed view, following querying."/>
-    <x v="6"/>
-    <s v="In progress"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="15"/>
-    <m/>
-    <m/>
-    <s v="The detailed view has a field called &quot;events&quot;, over flows on to other fields as the text of that field grows in the UI_x000a_2. &quot;prepration_type&quot; field is not shown in detailed view_x000a_3. cannot see fields, delete_by, updated_by,created_by,audited_by_x000a_3. updated_user fields never gets populated._x000a_4. write access field is available in API not here, what is it doing ?"/>
-    <s v="#112_x000a_#113_x000a_#114_x000a_#115"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
   </r>
   <r>
     <s v="R5A.34"/>
@@ -2967,7 +2971,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <m/>
     <m/>
@@ -2984,11 +2987,26 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <m/>
     <m/>
     <m/>
+  </r>
+  <r>
+    <s v="R5A.36"/>
+    <s v="The graphs in the dashboard view in the current version are very sensitive and can go to negative values, instead, the graphs should be adjusted to visualise the data present, and the ranges automatically be set to correspond with the data.[Want to keep the zoom in the graph – still there but now only on x axis – disabled for y_x000a_axis]"/>
+    <x v="6"/>
+    <s v="Completed"/>
+    <d v="2024-05-23T00:00:00"/>
+    <s v="23/06/2024 [refined on 10th June 2024]"/>
+    <m/>
+    <m/>
+    <m/>
+    <s v="#102"/>
+    <d v="2024-12-09T00:00:00"/>
+    <s v="Graph issue"/>
+    <m/>
+    <s v="Only sensitive in x axis"/>
   </r>
   <r>
     <s v="R5A.38"/>
@@ -3001,7 +3019,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-24T00:00:00"/>
     <m/>
     <m/>
@@ -3018,7 +3035,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <m/>
     <m/>
@@ -3035,58 +3051,38 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <d v="2024-09-06T00:00:00"/>
     <m/>
     <m/>
     <s v="Not sure if this a requirement"/>
   </r>
   <r>
-    <s v="R5A.01"/>
-    <s v="Users with write access can edit another user's asset groups (adding and removing assets, deleting the group, adding digitisers, etc.)"/>
+    <m/>
+    <s v=" After demo on 10June 2024, search result were not paginated so  requirement for pagination was added, along with possibility to select all search result across all pages."/>
     <x v="6"/>
-    <s v="In progress"/>
-    <d v="2024-08-01T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="10"/>
-    <m/>
-    <m/>
-    <s v="Not possible to share groups amongst users who haven't created assets"/>
-    <s v="#126"/>
-    <m/>
-    <s v="There is no admin role as of yet now, only read/write acccess - decided that."/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="R5A.02"/>
-    <s v="After performing a search, in case there are changes made to several fields, there is a confirmation of the action required by the user for that change to be applied. I can either confirm or cancel the change and only after that I can navigate away from that view. (Bulk Update)"/>
+    <s v="Completed"/>
+    <m/>
+    <d v="2024-06-10T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <s v=" search was requested to be Case insensitive search on fields without dropdown list"/>
     <x v="6"/>
-    <s v="In progress"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="10"/>
-    <m/>
-    <m/>
-    <s v="refer to issues in R5A.12A"/>
-    <s v="#129_x000a_#130_x000a__x000a_"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="To be able to perform correct mistakes or change initial metadata based on new information from UI"/>
-  </r>
-  <r>
-    <s v="R5A.04"/>
-    <s v="All metadata fields can be viewed in detailed view by all authorised users (read and write access)"/>
-    <x v="6"/>
-    <s v="In progress"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="5"/>
-    <m/>
-    <m/>
-    <s v="Write access in UI not available, cannot edit fields in UI"/>
-    <s v="#108_x000a_#113"/>
+    <s v="Completed"/>
+    <m/>
+    <d v="2024-06-10T00:00:00"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
     <m/>
     <m/>
     <m/>
@@ -3102,12 +3098,59 @@
     <n v="20"/>
     <n v="1"/>
     <m/>
-    <s v="1.Search functionality missing &quot;AND&quot; operator _x000a_2. NOT operator not available in search functionality_x000a_3.After using UI for a while, search starts to give incorrect/inconsistent results_x000a_4. Field &quot;asset_locked&quot; search doesn't work _x000a_5. In search functionality, file_formats search doesn't work._x000a_6. Result count of the search result missing_x000a_7.internal_status is also an enum but doesnt load as one._x000a_8.Wrong operator types for &quot;asset_updated_by&quot; field._x000a_9. Field &quot;asset_group&quot; search functionality not working _x000a_10.Search functionality not working for field &quot;restricted_access&quot;_x000a_11. Search functionality not find correct results for fields &quot;Workstation&quot; and &quot;Pipeline&quot;_x000a_12. Failed search query doesn't produce any errors_x000a_13. Search functionality missing for certain fields"/>
     <s v="#109_x000a_#110_x000a_#111_x000a_#116_x000a_#117_x000a_#119_x000a_#120_x000a_#121_x000a_#122_x000a_#123_x000a_#124_x000a_#125_x000a_#135"/>
     <m/>
-    <s v="Provides a programmable way (API) to query the graph database also. currently has a bug- provides incorrect result, see saved search."/>
+    <s v="Provides a programmable way (API) to query the graph database also. Currently has a bug- provides incorrect result, see saved search._x000a_1.Search functionality missing &quot;AND&quot; operator _x000a_2. NOT operator not available in search functionality_x000a_3.After using UI for a while, search starts to give incorrect/inconsistent results_x000a_4. Field &quot;asset_locked&quot; search doesn't work _x000a_5. In search functionality, file_formats search doesn't work._x000a_6. Result count of the search result missing_x000a_7.internal_status is also an enum but doesnt load as one._x000a_8.Wrong operator types for &quot;asset_updated_by&quot; field._x000a_9. Field &quot;asset_group&quot; search functionality not working _x000a_10.Search functionality not working for field &quot;restricted_access&quot;_x000a_11. Search functionality not find correct results for fields &quot;Workstation&quot; and &quot;Pipeline&quot;_x000a_12. Failed search query doesn't produce any errors_x000a_13. Search functionality missing for certain fields"/>
     <m/>
     <s v="Search UI for assets in the ARS to perform quality checks etc, in the demo on 10 June 2024 , one of AND or OR was missing is the search functionality and it was reiterated that there need to be both AND&amp;OR on node level search."/>
+  </r>
+  <r>
+    <s v="R5A.01"/>
+    <s v="Users with write access can edit another user's asset groups (adding and removing assets, deleting the group, adding digitisers, etc.)"/>
+    <x v="6"/>
+    <s v="In progress"/>
+    <d v="2024-08-01T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="10"/>
+    <m/>
+    <m/>
+    <s v="#126"/>
+    <m/>
+    <s v="There is no admin role as of yet now, only read/write acccess - decided that. Not possible to share groups amongst users who haven't created assets."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R5A.02"/>
+    <s v="After performing a search, in case there are changes made to several fields, there is a confirmation of the action required by the user for that change to be applied. I can either confirm or cancel the change and only after that I can navigate away from that view. (Bulk Update)"/>
+    <x v="6"/>
+    <s v="In progress"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="10"/>
+    <m/>
+    <m/>
+    <s v="#129_x000a_#130_x000a__x000a_"/>
+    <m/>
+    <s v="Refer to issues in R5A.12A"/>
+    <m/>
+    <s v="To be able to perform correct mistakes or change initial metadata based on new information from UI"/>
+  </r>
+  <r>
+    <s v="R5A.04"/>
+    <s v="All metadata fields can be viewed in detailed view by all authorised users (read and write access)"/>
+    <x v="6"/>
+    <s v="In progress"/>
+    <d v="2024-05-23T00:00:00"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <s v="#108_x000a_#113"/>
+    <m/>
+    <s v="Write access in UI not available, cannot edit fields in UI"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="R5A.07"/>
@@ -3119,10 +3162,9 @@
     <n v="15"/>
     <m/>
     <m/>
+    <s v="#108_x000a_#132"/>
+    <m/>
     <s v="Not possible to edit in detailed view"/>
-    <s v="#108_x000a_#132"/>
-    <m/>
-    <s v="works"/>
     <m/>
     <s v="Basic functionality of how read write works"/>
   </r>
@@ -3136,10 +3178,9 @@
     <n v="3"/>
     <m/>
     <m/>
+    <s v="#127_x000a_#128_x000a_"/>
+    <m/>
     <s v="1. Downloading CSV works, but events fields doesnt get populated in csv_x000a_2. Downloading images of single asset doesnt work."/>
-    <s v="#127_x000a_#128_x000a_"/>
-    <m/>
-    <m/>
     <m/>
     <s v="Both download the csv as well as the asset with images themselves as seperate functionality"/>
   </r>
@@ -3153,29 +3194,11 @@
     <n v="7"/>
     <m/>
     <m/>
-    <s v="Remove date range when querying this metadata field and replace with operator“=” "/>
     <s v="#120"/>
     <m/>
-    <s v="Covered as part of the search requirement using metadatafield &quot;updated by&quot;. not working."/>
+    <s v="Covered as part of the search requirement using metadatafield &quot;updated by&quot;. not working._x000a_Remove date range when querying this metadata field and replace with operator“=” "/>
     <m/>
     <s v="To be able to see latest changes in the system"/>
-  </r>
-  <r>
-    <s v="R5A.11"/>
-    <s v="In detailed view, it is possible to navigate back and forth through assets that have been retrieved as part of a search. "/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <d v="2024-09-24T00:00:00"/>
-    <m/>
-    <m/>
-    <s v="To see the search result in a sequence for inspection or other purposes"/>
   </r>
   <r>
     <s v="R5A.12A"/>
@@ -3187,29 +3210,11 @@
     <n v="7"/>
     <m/>
     <m/>
-    <s v="1.Seek clarification on why pipeline and workstation values are needed_x000a_2. Back and forward buttons when in a group donoto navigate in the group but instead correspodn to last query._x000a_"/>
     <s v="#129_x000a_#130_x000a__x000a_"/>
     <m/>
-    <s v="I think #130 is not covered in the requirement, does it read as a new requirement"/>
+    <s v="1.Seek clarification on why pipeline and workstation values are needed_x000a_2. Back and forward buttons when in a group don'to navigate in the group but instead correspond to last query._x000a_#130 possibly not covered in the requirement"/>
     <m/>
     <s v="Bulk update several record for the ease of correction after audit, the way bulk update is implemented is that it rewrites the existing values of the bulk updatable metadata fields, except tags which maintains the exisitng values and appends to the list.(10June 2024)"/>
-  </r>
-  <r>
-    <s v="R5A.13"/>
-    <s v="It is possible to create a group of asset records and add to this group with additional records later.  "/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <d v="2024-09-24T00:00:00"/>
-    <m/>
-    <m/>
-    <s v="To save search results and maintain/add to them for purpose of correction, bulk action, or similar"/>
   </r>
   <r>
     <s v="R5A.14"/>
@@ -3221,10 +3226,9 @@
     <n v="7"/>
     <m/>
     <m/>
-    <s v="1. Downloading metadata of multiple assets work, but events field doesn't get populated_x000a_2.Downloading images/media of multiple assets dont work."/>
     <s v="#131_x000a_#127"/>
-    <s v="related to R5A.9"/>
-    <m/>
+    <m/>
+    <s v="1. Downloading metadata of multiple assets work, but events field doesn't get populated_x000a_2.Downloading images/media of multiple assets dont work._x000a_Related to R5A.9"/>
     <m/>
     <m/>
   </r>
@@ -3238,10 +3242,9 @@
     <n v="7"/>
     <m/>
     <m/>
-    <s v="There is no functionality to download parent asset/acces related assets. I would expect to get the option to download parent/children asset(s) when aaplicable. How is this requirement fulfilled ?"/>
     <s v="#133"/>
-    <s v="related to R5A.9"/>
-    <s v="We are also trying to deploy graph db viewer which might need some expertise but can provide this functionality. This could be dropped. Recently downloading assets not working properly"/>
+    <m/>
+    <s v="There is no functionality to download parent asset/access related assets. I would expect to get the option to download parent/children asset(s) when applicable. How is this requirement fulfilled ?_x000a_We are also trying to deploy graph db viewer which might need some expertise but can provide this functionality. Recently downloading assets not working properly_x000a_Related to R5A.9"/>
     <m/>
     <s v="This can be covered by existing search functionality "/>
   </r>
@@ -3255,7 +3258,6 @@
     <n v="3"/>
     <m/>
     <m/>
-    <s v="graph issue"/>
     <s v="#102"/>
     <m/>
     <s v="Graphs not working properly, almost there"/>
@@ -3272,7 +3274,6 @@
     <n v="3"/>
     <m/>
     <m/>
-    <s v="graph issue"/>
     <s v="#102"/>
     <m/>
     <s v="Graphs not working properly,almost there "/>
@@ -3289,10 +3290,9 @@
     <n v="10"/>
     <m/>
     <m/>
+    <s v="#134"/>
+    <m/>
     <s v="Not able to search assets without media"/>
-    <s v="#134"/>
-    <m/>
-    <m/>
     <m/>
     <s v="Covererd by search functionality"/>
   </r>
@@ -3306,46 +3306,11 @@
     <n v="3"/>
     <m/>
     <m/>
-    <s v="refer to bugs in R5.14 and R5A.06"/>
-    <m/>
-    <m/>
-    <m/>
+    <m/>
+    <m/>
+    <s v="Refer to bugs in R5.14 and R5A.06"/>
     <m/>
     <s v="Covered by search functionality"/>
-  </r>
-  <r>
-    <s v="R5A.24"/>
-    <s v="It should be possible to assign either write or read only access to pre-defined users of ARS, who are able to log in and view records using the UI"/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="3"/>
-    <m/>
-    <m/>
-    <s v="graph issue"/>
-    <s v="#102"/>
-    <d v="2024-12-09T00:00:00"/>
-    <s v="works"/>
-    <m/>
-    <s v="Allow a limited number of people to use it and try it out (due to lack of may security features most people will have only read access)"/>
-  </r>
-  <r>
-    <s v="R5A.25"/>
-    <s v="It should be possible to download graphs and statistics in the dashboard view as reports and PDFs/editable documents. "/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <d v="2024-05-23T00:00:00"/>
-    <d v="2024-06-23T00:00:00"/>
-    <n v="3"/>
-    <m/>
-    <m/>
-    <s v="graph issue"/>
-    <s v="#102"/>
-    <d v="2024-12-09T00:00:00"/>
-    <s v="works"/>
-    <m/>
-    <s v="Exisitng functionality, updated to support new features"/>
   </r>
   <r>
     <s v="R5A.26"/>
@@ -3357,10 +3322,9 @@
     <n v="20"/>
     <m/>
     <m/>
-    <s v="has quirks like workstation and pipeline are mandatory fields meaning it is not possible to bulk update assets from different work station, pipeline"/>
     <s v="#129_x000a_#130_x000a__x000a_"/>
     <m/>
-    <s v="Bulk update works, has quirks like workstation and pipeline are mandatory fields meaning it is not possible to bulk update assets from different work station, pipeline"/>
+    <s v="Bulk update works, has quirks like workstation and pipeline are mandatory fields meaning it is not possible to bulk update assets from different work station, pipeline."/>
     <m/>
     <s v="Bulk update- not sure if compare function was postponed?"/>
   </r>
@@ -3374,10 +3338,9 @@
     <n v="2"/>
     <m/>
     <m/>
+    <s v="#132"/>
+    <m/>
     <s v="1. it is not possible to download asset media_x000a_2. It is not possible to edit metadata except through bulk update."/>
-    <s v="#132"/>
-    <m/>
-    <m/>
     <m/>
     <s v="Went back and forth "/>
   </r>
@@ -3391,29 +3354,27 @@
     <n v="3"/>
     <m/>
     <m/>
-    <s v="not working "/>
     <s v="#132"/>
-    <s v="related to R5A.9"/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="R5A.36"/>
-    <s v="The graphs in the dashboard view in the current version are very sensitive and can go to negative values, instead, the graphs should be adjusted to visualise the data present, and the ranges automatically be set to correspond with the data.[Want to keep the zoom in the graph – still there but now only on x axis – disabled for y_x000a_axis]"/>
+    <m/>
+    <s v="Not working _x000a_Related to R5A.9"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="R5A.33"/>
+    <s v="The assets are visible in the UI in the form of both a list view and detailed view, following querying."/>
     <x v="6"/>
-    <s v="Completed"/>
+    <s v="In progress"/>
     <d v="2024-05-23T00:00:00"/>
-    <s v="23/06/2024 [refined on 10th June 2024]"/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="graph issue"/>
-    <s v="#102"/>
-    <d v="2024-12-09T00:00:00"/>
-    <s v="Works"/>
-    <m/>
-    <s v="Only sensitive in x axis"/>
+    <d v="2024-06-23T00:00:00"/>
+    <n v="15"/>
+    <m/>
+    <m/>
+    <s v="#112_x000a_#113_x000a_#114_x000a_#115"/>
+    <m/>
+    <s v="The detailed view has a field called &quot;events&quot;, over flows on to other fields as the text of that field grows in the UI_x000a_2. &quot;prepration_type&quot; field is not shown in detailed view_x000a_3. cannot see fields, delete_by, updated_by,created_by,audited_by_x000a_3. updated_user fields never gets populated._x000a_4. write access field is available in API not here, what is it doing ?"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="R5A.39"/>
@@ -3425,10 +3386,9 @@
     <n v="5"/>
     <m/>
     <m/>
-    <s v="issues in R5.06 are related to this - Field &quot;internal_status&quot; doesnot have a dropdown"/>
     <s v="#119"/>
     <m/>
-    <s v="Missing date for decision- was 10th June 2024. needs more thorough testing"/>
+    <s v="Issues in R5.06 are related to this - Field &quot;internal_status&quot; does not have a dropdown_x000a_Needs more thorough testing."/>
     <m/>
     <s v="Later decides, some fo the fields will be cached, provided a list"/>
   </r>
@@ -3442,12 +3402,27 @@
     <n v="3"/>
     <m/>
     <m/>
-    <s v="graph issue"/>
     <s v="#102"/>
     <m/>
-    <m/>
+    <s v="Graph issue"/>
     <n v="1"/>
     <s v="Satisfied with previous functionality"/>
+  </r>
+  <r>
+    <m/>
+    <s v="can share links of the graphs with custom date ranges so others will have the same view of the graph as you."/>
+    <x v="6"/>
+    <s v="In progress"/>
+    <m/>
+    <d v="2024-06-17T00:00:00"/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <s v="#102"/>
+    <m/>
+    <s v="Not tested, graph not working"/>
+    <m/>
+    <m/>
   </r>
   <r>
     <s v="R5A.23"/>
@@ -3461,7 +3436,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Why was this removed?- partially covered in events protocol"/>
     <m/>
     <s v="Basic functionality saving data"/>
@@ -3471,7 +3445,6 @@
     <s v="The reports and graphs in dashboard view along with their data are downloadable"/>
     <x v="6"/>
     <s v="Removed"/>
-    <m/>
     <m/>
     <m/>
     <m/>
@@ -3495,7 +3468,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Needs more thorough testing"/>
     <m/>
     <s v="Postponed"/>
@@ -3505,7 +3477,6 @@
     <s v="It should be possible to view the various related (derivates, original) images of the asset in the detailed view"/>
     <x v="7"/>
     <s v="Not started"/>
-    <m/>
     <m/>
     <m/>
     <m/>
@@ -3529,7 +3500,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Delayed to next work package - date for decision missing. was postponed to next iteration -decsion date missing"/>
     <m/>
     <s v="To be able to sort fields to view data in a certain order in the search view"/>
@@ -3546,7 +3516,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Delayed to next work package - date for decision missing. needs more thorough testing"/>
     <m/>
     <s v="Admin role, who can create and manage access, like project leader or technical lead to provide access to internal/external users, etc. On request, for now only read and write access can be provided based on access request via keycloak"/>
@@ -3563,7 +3532,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="postponed - decision date missing"/>
     <m/>
     <s v="View the asset"/>
@@ -3582,7 +3550,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Postponed"/>
   </r>
   <r>
@@ -3597,7 +3564,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="You can ascend/descend the institution, collection, barcodes fileformats, created date"/>
     <m/>
     <s v="Postponed"/>
@@ -3614,7 +3580,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Institution and collection implemented in 5A, asset level remaining"/>
     <m/>
     <m/>
@@ -3631,7 +3596,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Not directly available on dashboard but available through search "/>
     <m/>
     <m/>
@@ -3648,7 +3612,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Audited_by fields provides that info but cannot be edited in 5A as of yet and search field for search for audited assets"/>
     <m/>
     <m/>
@@ -3665,7 +3628,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="End point available but not in UI"/>
     <m/>
     <m/>
@@ -3685,7 +3647,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R5B.06"/>
@@ -3702,7 +3663,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R5B.07"/>
@@ -3719,7 +3679,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R5B.08"/>
@@ -3736,7 +3695,6 @@
     <m/>
     <m/>
     <m/>
-    <m/>
   </r>
   <r>
     <s v="R5B.09"/>
@@ -3752,6 +3710,37 @@
     <m/>
     <m/>
     <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <s v="Be able to see all the open shares in the file proxy - i.e., the precise status list shown. See notes for R1.14, GET list shares end point to include status"/>
+    <x v="8"/>
+    <s v="In progress"/>
+    <d v="2024-11-20T00:00:00"/>
+    <m/>
+    <n v="10"/>
+    <n v="1"/>
+    <m/>
+    <s v="#107"/>
+    <m/>
+    <s v="Related to R1.14, the requirement mentions that status should also be presented, so it is missing functionality of R1.14"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <s v="When a derivative asset needs to be created in the ARS, the parent GUID should be filled in (as sent by integration server) for both jpegs and tifs"/>
+    <x v="8"/>
+    <s v="In progress"/>
+    <m/>
+    <m/>
+    <n v="20"/>
+    <n v="1"/>
+    <m/>
+    <s v="#125"/>
+    <m/>
+    <s v="Missing parent GUID issue"/>
     <m/>
     <m/>
   </r>
@@ -3767,27 +3756,9 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Has issues like needs asset pid to create metadata, to do after metadata discussion completed"/>
     <m/>
     <s v="From previous version, not detailed here"/>
-  </r>
-  <r>
-    <m/>
-    <s v="Be able to see all the open shares in the file proxy - i.e., the precise status list shown. See notes for R1.14, GET list shares end point to include status"/>
-    <x v="8"/>
-    <s v="In progress"/>
-    <d v="2024-11-20T00:00:00"/>
-    <m/>
-    <n v="10"/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <s v="#107"/>
-    <m/>
-    <s v="Related to R1.14, the requirement mentions that status should also be presented, so it is missing functionality of R1.14"/>
-    <m/>
-    <m/>
   </r>
   <r>
     <m/>
@@ -3801,118 +3772,14 @@
     <m/>
     <m/>
     <m/>
-    <m/>
     <s v="Status field is not being used for anything, It would be heæpful to know the statu so f asset when someone other than integration server creates an asset or other similar use cases, look at metadata spreadsheet, should user field also be mandatory? To do after metadata discussion completed"/>
     <m/>
     <m/>
   </r>
   <r>
     <m/>
-    <s v="When a derivative asset needs to be created in the ARS, the parent GUID should be filled in (as sent by integration server) for both jpegs and tifs"/>
-    <x v="8"/>
-    <s v="In progress"/>
-    <m/>
-    <m/>
-    <n v="20"/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <s v="#125"/>
-    <m/>
-    <s v="Missing parent GUID issue"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="R3.19"/>
-    <s v="Provide granular control over access at  institution and collection level. "/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <d v="2024-05-30T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <d v="2024-12-09T00:00:00"/>
-    <s v="Documentation of this is  https://github.com/NHMDenmark/DaSSCo-asset-service/issues/100, needs testing by us"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <s v="R3.20"/>
-    <s v="Deploy test suite"/>
-    <x v="1"/>
-    <s v="Not started"/>
-    <d v="2024-11-20T00:00:00"/>
-    <m/>
-    <n v="10"/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <s v="#105_x000a_#106"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <s v=" After demo on 10June 2024, search result were not paginated so  requirement for pagination was added, along with possibility to select all search result across all pages."/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <m/>
-    <d v="2024-06-10T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <s v="can share links of the graphs with custom date ranges so others will have the same view of the graph as you."/>
-    <x v="6"/>
-    <s v="In progress"/>
-    <m/>
-    <d v="2024-06-17T00:00:00"/>
-    <n v="3"/>
-    <m/>
-    <m/>
-    <s v="graph issue"/>
-    <s v="#102"/>
-    <m/>
-    <s v="not tested, graph not working"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <s v=" search was requested to be Case insensitive search on fields without dropdown list"/>
-    <x v="6"/>
-    <s v="Completed"/>
-    <m/>
-    <d v="2024-06-10T00:00:00"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
     <m/>
     <x v="9"/>
-    <m/>
     <m/>
     <m/>
     <m/>
@@ -3929,9 +3796,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CC338E7-EB0F-4F57-B992-9C99252CD269}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CC338E7-EB0F-4F57-B992-9C99252CD269}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="15">
+  <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -3953,7 +3820,6 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -4342,7 +4208,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7660,7 +7526,7 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7681,7 +7547,7 @@
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="21">
         <v>19</v>
       </c>
     </row>
@@ -7689,7 +7555,7 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="21">
         <v>84</v>
       </c>
     </row>
@@ -7697,12 +7563,13 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
+      <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="21">
         <v>194</v>
       </c>
     </row>
@@ -7710,17 +7577,19 @@
       <c r="A8" s="3" t="s">
         <v>126</v>
       </c>
+      <c r="B8" s="21"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="21">
         <v>167</v>
       </c>
     </row>
@@ -7728,12 +7597,13 @@
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="B11" s="21"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="21">
         <v>46</v>
       </c>
     </row>
@@ -7741,12 +7611,13 @@
       <c r="A13" s="3" t="s">
         <v>165</v>
       </c>
+      <c r="B13" s="21"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="21">
         <v>510</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusting ARS Phase 3 time estimates.
</commit_message>
<xml_diff>
--- a/Asset Registry System (ARS)/ARS Requirements Phase 3 work_V22.xlsx
+++ b/Asset Registry System (ARS)/ARS Requirements Phase 3 work_V22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/btw897_ku_dk/Documents/DaSSCo-Tranche-1-work/Asset Registry System (ARS)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimstp/Documents/NHMD/docs/DaSSCo/github/DaSSCo-Tranche-1-work/Asset Registry System (ARS)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{B245CD1A-D358-4CAE-8D69-48AFBC9E5966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{080665FF-1590-4471-9091-ABB85DE98B24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508BEC1D-E515-0242-A61C-77C57AE15F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{E45C9BED-A893-4BAC-8B4F-82BC01806C6A}"/>
+    <workbookView xWindow="3440" yWindow="2280" windowWidth="27220" windowHeight="14280" xr2:uid="{E45C9BED-A893-4BAC-8B4F-82BC01806C6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1527,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1585,7 +1585,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3796,7 +3795,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CC338E7-EB0F-4F57-B992-9C99252CD269}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CC338E7-EB0F-4F57-B992-9C99252CD269}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -4205,31 +4204,31 @@
   <dimension ref="A1:P131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="4" customWidth="1"/>
-    <col min="2" max="2" width="48.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" style="6" customWidth="1"/>
-    <col min="7" max="10" width="10.81640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="36.81640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="47.36328125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="24.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.81640625" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="8.6328125" style="4"/>
+    <col min="4" max="4" width="18.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="6" customWidth="1"/>
+    <col min="7" max="10" width="10.83203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="6" customWidth="1"/>
+    <col min="12" max="12" width="36.83203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="47.33203125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.83203125" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -4273,7 +4272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
@@ -4308,7 +4307,7 @@
       </c>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>64</v>
       </c>
@@ -4337,7 +4336,7 @@
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>286</v>
       </c>
@@ -4359,7 +4358,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>287</v>
       </c>
@@ -4381,7 +4380,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" ht="105.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="105.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>285</v>
       </c>
@@ -4405,7 +4404,7 @@
       </c>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>288</v>
       </c>
@@ -4429,7 +4428,7 @@
       </c>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>289</v>
       </c>
@@ -4453,7 +4452,7 @@
       </c>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>290</v>
       </c>
@@ -4480,7 +4479,7 @@
       </c>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>291</v>
       </c>
@@ -4507,7 +4506,7 @@
       </c>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>292</v>
       </c>
@@ -4534,7 +4533,7 @@
       </c>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -4559,7 +4558,7 @@
       </c>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:15" ht="113" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="113" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>62</v>
       </c>
@@ -4585,7 +4584,7 @@
       </c>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -4613,7 +4612,7 @@
       </c>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:15" ht="71" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="71" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
@@ -4638,7 +4637,7 @@
       </c>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:15" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>67</v>
       </c>
@@ -4666,7 +4665,7 @@
       </c>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
@@ -4694,7 +4693,7 @@
       </c>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:16" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
@@ -4719,7 +4718,7 @@
       </c>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>103</v>
       </c>
@@ -4745,7 +4744,7 @@
       <c r="O19" s="9"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="1:16" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
@@ -4779,7 +4778,7 @@
       </c>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:16" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>69</v>
       </c>
@@ -4812,7 +4811,7 @@
       </c>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
@@ -4849,7 +4848,7 @@
       </c>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>294</v>
       </c>
@@ -4876,7 +4875,7 @@
       </c>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:16" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>298</v>
       </c>
@@ -4903,7 +4902,7 @@
       </c>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="1:16" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>119</v>
       </c>
@@ -4930,7 +4929,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>195</v>
       </c>
@@ -4957,7 +4956,7 @@
       </c>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>120</v>
       </c>
@@ -4984,7 +4983,7 @@
       </c>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>121</v>
       </c>
@@ -5011,7 +5010,7 @@
       </c>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>293</v>
       </c>
@@ -5052,7 +5051,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>295</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>299</v>
       </c>
@@ -5115,7 +5114,7 @@
       </c>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" spans="1:16" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>122</v>
       </c>
@@ -5143,7 +5142,7 @@
       </c>
       <c r="O32" s="9"/>
     </row>
-    <row r="33" spans="1:16" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>124</v>
       </c>
@@ -5171,7 +5170,7 @@
       </c>
       <c r="O33" s="9"/>
     </row>
-    <row r="34" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>296</v>
       </c>
@@ -5201,7 +5200,7 @@
       </c>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>123</v>
       </c>
@@ -5225,7 +5224,7 @@
       </c>
       <c r="O35" s="9"/>
     </row>
-    <row r="36" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>277</v>
       </c>
@@ -5255,7 +5254,7 @@
       <c r="N36" s="8"/>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>125</v>
       </c>
@@ -5277,7 +5276,7 @@
       <c r="K37" s="4"/>
       <c r="O37" s="9"/>
     </row>
-    <row r="38" spans="1:16" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>118</v>
       </c>
@@ -5299,7 +5298,7 @@
       </c>
       <c r="O38" s="9"/>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>297</v>
       </c>
@@ -5320,7 +5319,7 @@
       </c>
       <c r="O39" s="9"/>
     </row>
-    <row r="40" spans="1:16" ht="145" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>195</v>
       </c>
@@ -5348,7 +5347,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="8"/>
     </row>
-    <row r="41" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>300</v>
       </c>
@@ -5363,7 +5362,7 @@
       </c>
       <c r="O41" s="9"/>
     </row>
-    <row r="42" spans="1:16" s="8" customFormat="1" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" s="8" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>301</v>
       </c>
@@ -5389,7 +5388,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>302</v>
       </c>
@@ -5404,7 +5403,7 @@
       </c>
       <c r="O43" s="9"/>
     </row>
-    <row r="44" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>303</v>
       </c>
@@ -5419,7 +5418,7 @@
       </c>
       <c r="O44" s="9"/>
     </row>
-    <row r="45" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>304</v>
       </c>
@@ -5434,7 +5433,7 @@
       </c>
       <c r="O45" s="9"/>
     </row>
-    <row r="46" spans="1:16" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>305</v>
       </c>
@@ -5449,7 +5448,7 @@
       </c>
       <c r="O46" s="9"/>
     </row>
-    <row r="47" spans="1:16" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>306</v>
       </c>
@@ -5464,7 +5463,7 @@
       </c>
       <c r="O47" s="9"/>
     </row>
-    <row r="48" spans="1:16" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>307</v>
       </c>
@@ -5479,7 +5478,7 @@
       </c>
       <c r="O48" s="9"/>
     </row>
-    <row r="49" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>308</v>
       </c>
@@ -5503,7 +5502,7 @@
       </c>
       <c r="O49" s="9"/>
     </row>
-    <row r="50" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>309</v>
       </c>
@@ -5527,7 +5526,7 @@
       </c>
       <c r="O50" s="9"/>
     </row>
-    <row r="51" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>310</v>
       </c>
@@ -5548,7 +5547,7 @@
       </c>
       <c r="O51" s="9"/>
     </row>
-    <row r="52" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>311</v>
       </c>
@@ -5569,7 +5568,7 @@
       </c>
       <c r="O52" s="9"/>
     </row>
-    <row r="53" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>312</v>
       </c>
@@ -5594,7 +5593,7 @@
       <c r="N53" s="11"/>
       <c r="O53" s="9"/>
     </row>
-    <row r="54" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>313</v>
       </c>
@@ -5615,7 +5614,7 @@
       </c>
       <c r="O54" s="9"/>
     </row>
-    <row r="55" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>316</v>
       </c>
@@ -5636,7 +5635,7 @@
       </c>
       <c r="O55" s="9"/>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>314</v>
       </c>
@@ -5657,7 +5656,7 @@
       </c>
       <c r="O56" s="9"/>
     </row>
-    <row r="57" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>315</v>
       </c>
@@ -5681,7 +5680,7 @@
       </c>
       <c r="O57" s="9"/>
     </row>
-    <row r="58" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>317</v>
       </c>
@@ -5696,7 +5695,7 @@
       </c>
       <c r="O58" s="9"/>
     </row>
-    <row r="59" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>317</v>
       </c>
@@ -5711,7 +5710,7 @@
       </c>
       <c r="O59" s="9"/>
     </row>
-    <row r="60" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>317</v>
       </c>
@@ -5726,7 +5725,7 @@
       </c>
       <c r="O60" s="9"/>
     </row>
-    <row r="61" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>317</v>
       </c>
@@ -5741,7 +5740,7 @@
       </c>
       <c r="O61" s="9"/>
     </row>
-    <row r="62" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>317</v>
       </c>
@@ -5756,7 +5755,7 @@
       </c>
       <c r="O62" s="9"/>
     </row>
-    <row r="63" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>317</v>
       </c>
@@ -5771,7 +5770,7 @@
       </c>
       <c r="O63" s="9"/>
     </row>
-    <row r="64" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>317</v>
       </c>
@@ -5786,7 +5785,7 @@
       </c>
       <c r="O64" s="9"/>
     </row>
-    <row r="65" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>318</v>
       </c>
@@ -5801,7 +5800,7 @@
       </c>
       <c r="O65" s="9"/>
     </row>
-    <row r="66" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>319</v>
       </c>
@@ -5816,7 +5815,7 @@
       </c>
       <c r="O66" s="9"/>
     </row>
-    <row r="67" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>320</v>
       </c>
@@ -5831,7 +5830,7 @@
       </c>
       <c r="O67" s="9"/>
     </row>
-    <row r="68" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>321</v>
       </c>
@@ -5846,7 +5845,7 @@
       </c>
       <c r="O68" s="9"/>
     </row>
-    <row r="69" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>322</v>
       </c>
@@ -5861,7 +5860,7 @@
       </c>
       <c r="O69" s="9"/>
     </row>
-    <row r="70" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>323</v>
       </c>
@@ -5876,7 +5875,7 @@
       </c>
       <c r="O70" s="9"/>
     </row>
-    <row r="71" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>324</v>
       </c>
@@ -5891,7 +5890,7 @@
       </c>
       <c r="O71" s="9"/>
     </row>
-    <row r="72" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>276</v>
       </c>
@@ -5919,7 +5918,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>74</v>
       </c>
@@ -5945,7 +5944,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>75</v>
       </c>
@@ -5971,7 +5970,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>79</v>
       </c>
@@ -5994,7 +5993,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>83</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>85</v>
       </c>
@@ -6058,7 +6057,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>86</v>
       </c>
@@ -6093,7 +6092,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>89</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>91</v>
       </c>
@@ -6139,7 +6138,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>93</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>94</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>95</v>
       </c>
@@ -6218,7 +6217,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="409" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" ht="409" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>97</v>
       </c>
@@ -6241,7 +6240,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>100</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>101</v>
       </c>
@@ -6287,7 +6286,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>372</v>
       </c>
@@ -6303,7 +6302,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="9"/>
     </row>
-    <row r="88" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" s="4" t="s">
         <v>376</v>
       </c>
@@ -6318,7 +6317,7 @@
       </c>
       <c r="J88" s="9"/>
     </row>
-    <row r="89" spans="1:15" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>325</v>
       </c>
@@ -6353,7 +6352,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>282</v>
       </c>
@@ -6382,7 +6381,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>283</v>
       </c>
@@ -6414,7 +6413,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>284</v>
       </c>
@@ -6443,7 +6442,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>326</v>
       </c>
@@ -6478,7 +6477,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>327</v>
       </c>
@@ -6510,7 +6509,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>73</v>
       </c>
@@ -6542,7 +6541,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>340</v>
       </c>
@@ -6574,7 +6573,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>76</v>
       </c>
@@ -6603,7 +6602,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>77</v>
       </c>
@@ -6635,7 +6634,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>78</v>
       </c>
@@ -6667,7 +6666,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>80</v>
       </c>
@@ -6699,7 +6698,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>81</v>
       </c>
@@ -6731,7 +6730,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>82</v>
       </c>
@@ -6761,7 +6760,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>87</v>
       </c>
@@ -6793,7 +6792,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>88</v>
       </c>
@@ -6825,7 +6824,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>90</v>
       </c>
@@ -6854,7 +6853,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:14" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>92</v>
       </c>
@@ -6883,7 +6882,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:14" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>98</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>99</v>
       </c>
@@ -6950,7 +6949,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
         <v>374</v>
       </c>
@@ -6973,7 +6972,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:14" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>84</v>
       </c>
@@ -6999,7 +6998,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:14" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>96</v>
       </c>
@@ -7020,7 +7019,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:14" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>212</v>
       </c>
@@ -7043,7 +7042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>212</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>212</v>
       </c>
@@ -7086,7 +7085,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>212</v>
       </c>
@@ -7109,7 +7108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>212</v>
       </c>
@@ -7132,7 +7131,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>102</v>
       </c>
@@ -7150,7 +7149,7 @@
       </c>
       <c r="O117" s="9"/>
     </row>
-    <row r="118" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>212</v>
       </c>
@@ -7170,7 +7169,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>328</v>
       </c>
@@ -7188,7 +7187,7 @@
       </c>
       <c r="O119" s="9"/>
     </row>
-    <row r="120" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>329</v>
       </c>
@@ -7206,7 +7205,7 @@
       </c>
       <c r="O120" s="9"/>
     </row>
-    <row r="121" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>330</v>
       </c>
@@ -7224,7 +7223,7 @@
       </c>
       <c r="O121" s="9"/>
     </row>
-    <row r="122" spans="1:15" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>331</v>
       </c>
@@ -7242,7 +7241,7 @@
       </c>
       <c r="O122" s="9"/>
     </row>
-    <row r="123" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>332</v>
       </c>
@@ -7257,7 +7256,7 @@
       </c>
       <c r="O123" s="9"/>
     </row>
-    <row r="124" spans="1:15" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>333</v>
       </c>
@@ -7272,7 +7271,7 @@
       </c>
       <c r="O124" s="9"/>
     </row>
-    <row r="125" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>334</v>
       </c>
@@ -7287,7 +7286,7 @@
       </c>
       <c r="O125" s="9"/>
     </row>
-    <row r="126" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>335</v>
       </c>
@@ -7302,7 +7301,7 @@
       </c>
       <c r="O126" s="9"/>
     </row>
-    <row r="127" spans="1:15" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>336</v>
       </c>
@@ -7317,7 +7316,7 @@
       </c>
       <c r="O127" s="9"/>
     </row>
-    <row r="128" spans="1:15" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" s="4" t="s">
         <v>363</v>
       </c>
@@ -7347,7 +7346,7 @@
       <c r="N128" s="14"/>
       <c r="O128" s="15"/>
     </row>
-    <row r="129" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" s="4" t="s">
         <v>182</v>
       </c>
@@ -7374,7 +7373,7 @@
       <c r="N129" s="14"/>
       <c r="O129" s="15"/>
     </row>
-    <row r="130" spans="1:15" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>337</v>
       </c>
@@ -7406,7 +7405,7 @@
       </c>
       <c r="O130" s="15"/>
     </row>
-    <row r="131" spans="1:15" ht="116" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
         <v>181</v>
       </c>
@@ -7435,7 +7434,7 @@
   <autoFilter ref="A1:O131" xr:uid="{8DC291D6-8C8D-4010-87BA-D162CD1217BE}">
     <filterColumn colId="2">
       <filters>
-        <filter val="5A"/>
+        <filter val="2A"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -7529,13 +7528,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>163</v>
       </c>
@@ -7543,81 +7542,76 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7">
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="21"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="21"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="21"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="21"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14">
         <v>510</v>
       </c>
     </row>
@@ -7634,32 +7628,32 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -7676,7 +7670,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>